<commit_message>
2nd commit on 13 dec
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="11415" windowHeight="8955" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="11415" windowHeight="8955"/>
   </bookViews>
   <sheets>
-    <sheet name="testAddCustomer" sheetId="1" r:id="rId1"/>
-    <sheet name="testOpenAccount" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="testSuite" sheetId="3" r:id="rId1"/>
+    <sheet name="testAddCustomer" sheetId="1" r:id="rId2"/>
+    <sheet name="testOpenAccount" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="43">
   <si>
     <t>FirstName</t>
   </si>
@@ -121,6 +121,30 @@
   </si>
   <si>
     <t>3N4N1N</t>
+  </si>
+  <si>
+    <t>TC ID</t>
+  </si>
+  <si>
+    <t>RunMode</t>
+  </si>
+  <si>
+    <t>TestLoginAsBankManager</t>
+  </si>
+  <si>
+    <t>TestAddCustomer</t>
+  </si>
+  <si>
+    <t>TestOpenAccount</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>n</t>
   </si>
 </sst>
 </file>
@@ -452,6 +476,56 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="23.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -578,12 +652,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L11" sqref="G11:L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -675,16 +749,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
2nd commit on 15 dec
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -4,20 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="11415" windowHeight="8955" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="11415" windowHeight="8955" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="testSuite" sheetId="3" r:id="rId1"/>
     <sheet name="testAddCustomer" sheetId="1" r:id="rId2"/>
     <sheet name="testOpenAccount" sheetId="2" r:id="rId3"/>
-    <sheet name="Sheet1" r:id="rId8" sheetId="4"/>
+    <sheet name="testDeleteCustomer" r:id="rId8" sheetId="4"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="74">
   <si>
     <t>FirstName</t>
   </si>
@@ -151,61 +151,79 @@
     <t>Account Number</t>
   </si>
   <si>
+    <t>Granger</t>
+  </si>
+  <si>
+    <t>E859AB</t>
+  </si>
+  <si>
+    <t>1001 1002 1003</t>
+  </si>
+  <si>
+    <t>Harry</t>
+  </si>
+  <si>
+    <t>Potter</t>
+  </si>
+  <si>
+    <t>E725JB</t>
+  </si>
+  <si>
+    <t>1004 1005 1006</t>
+  </si>
+  <si>
+    <t>Weasly</t>
+  </si>
+  <si>
+    <t>E55555</t>
+  </si>
+  <si>
+    <t>1007 1008 1009</t>
+  </si>
+  <si>
+    <t>Albus</t>
+  </si>
+  <si>
+    <t>Dumbledore</t>
+  </si>
+  <si>
+    <t>E55656</t>
+  </si>
+  <si>
+    <t>1010 1011 1012</t>
+  </si>
+  <si>
+    <t>Neville</t>
+  </si>
+  <si>
+    <t>E89898</t>
+  </si>
+  <si>
+    <t>1013 1014 1015</t>
+  </si>
+  <si>
+    <t>Runmode</t>
+  </si>
+  <si>
+    <t>Delete Customer</t>
+  </si>
+  <si>
+    <t>Longbottom</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>testDeleteCustomer</t>
+  </si>
+  <si>
     <t>Hermoine</t>
   </si>
   <si>
-    <t>Granger</t>
-  </si>
-  <si>
-    <t>E859AB</t>
-  </si>
-  <si>
-    <t>1001 1002 1003</t>
-  </si>
-  <si>
-    <t>Harry</t>
-  </si>
-  <si>
-    <t>Potter</t>
-  </si>
-  <si>
-    <t>E725JB</t>
-  </si>
-  <si>
-    <t>1004 1005 1006</t>
-  </si>
-  <si>
     <t>Ron</t>
   </si>
   <si>
-    <t>Weasly</t>
-  </si>
-  <si>
-    <t>E55555</t>
-  </si>
-  <si>
-    <t>1007 1008 1009</t>
-  </si>
-  <si>
-    <t>Albus</t>
-  </si>
-  <si>
-    <t>Dumbledore</t>
-  </si>
-  <si>
-    <t>E55656</t>
-  </si>
-  <si>
-    <t>1010 1011 1012</t>
-  </si>
-  <si>
-    <t>Neville</t>
-  </si>
-  <si>
-    <t>Longbottom</t>
-  </si>
-  <si>
-    <t>E89898</t>
+    <t>1016 1022</t>
   </si>
   <si>
     <t>1017 1020</t>
@@ -217,19 +235,10 @@
     <t>1019</t>
   </si>
   <si>
-    <t>1013 1014 1015</t>
-  </si>
-  <si>
-    <t>Runmode</t>
-  </si>
-  <si>
-    <t>n</t>
-  </si>
-  <si>
-    <t>1016 1021</t>
-  </si>
-  <si>
-    <t>1022</t>
+    <t>1021</t>
+  </si>
+  <si>
+    <t>1023</t>
   </si>
 </sst>
 </file>
@@ -276,12 +285,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
@@ -580,10 +601,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -631,6 +652,14 @@
         <v>38</v>
       </c>
     </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -640,8 +669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -660,7 +689,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -730,7 +759,7 @@
         <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>68</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -744,7 +773,7 @@
         <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>68</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -785,7 +814,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C2" sqref="C2:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -868,7 +897,7 @@
         <v>28</v>
       </c>
       <c r="C7" t="s">
-        <v>68</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -879,7 +908,7 @@
         <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>68</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -911,7 +940,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -921,90 +950,103 @@
     <col min="2" max="2" bestFit="true" customWidth="true" width="12.23828125" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="10.01171875" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="16.2265625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="16.12109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s" s="5">
+      <c r="A1" t="s" s="16">
         <v>40</v>
       </c>
-      <c r="B1" t="s" s="6">
+      <c r="B1" t="s" s="17">
         <v>41</v>
       </c>
-      <c r="C1" t="s" s="7">
+      <c r="C1" t="s" s="18">
         <v>42</v>
       </c>
-      <c r="D1" t="s" s="8">
+      <c r="D1" t="s" s="19">
         <v>43</v>
+      </c>
+      <c r="E1" t="s" s="20">
+        <v>62</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" t="s">
         <v>44</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>45</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>46</v>
       </c>
-      <c r="D2" t="s">
-        <v>47</v>
+      <c r="E2" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" t="s">
         <v>48</v>
       </c>
-      <c r="B3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>50</v>
       </c>
-      <c r="D3" t="s">
-        <v>51</v>
+      <c r="E3" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" t="s">
         <v>52</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
         <v>53</v>
       </c>
-      <c r="C4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D4" t="s">
-        <v>55</v>
+      <c r="E4" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" t="s">
         <v>56</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D5" t="s">
         <v>57</v>
       </c>
-      <c r="C5" t="s">
-        <v>58</v>
-      </c>
-      <c r="D5" t="s">
-        <v>59</v>
+      <c r="E5" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" t="s">
         <v>60</v>
       </c>
-      <c r="B6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C6" t="s">
-        <v>62</v>
-      </c>
-      <c r="D6" t="s">
-        <v>66</v>
+      <c r="E6" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="7">
@@ -1018,7 +1060,10 @@
         <v>9</v>
       </c>
       <c r="D7" t="s">
-        <v>69</v>
+        <v>68</v>
+      </c>
+      <c r="E7" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="8">
@@ -1032,7 +1077,10 @@
         <v>10</v>
       </c>
       <c r="D8" t="s">
-        <v>63</v>
+        <v>69</v>
+      </c>
+      <c r="E8" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="9">
@@ -1046,6 +1094,9 @@
         <v>14</v>
       </c>
       <c r="D9" t="s">
+        <v>70</v>
+      </c>
+      <c r="E9" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1060,21 +1111,44 @@
         <v>11</v>
       </c>
       <c r="D10" t="s">
-        <v>65</v>
+        <v>71</v>
+      </c>
+      <c r="E10" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" t="s">
+        <v>72</v>
+      </c>
+      <c r="E11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
         <v>29</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>7</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C12" t="s">
         <v>31</v>
       </c>
-      <c r="D11" t="s">
-        <v>70</v>
+      <c r="D12" t="s">
+        <v>73</v>
+      </c>
+      <c r="E12" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1st commit on 15 dec
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="11415" windowHeight="8955"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="11415" windowHeight="8955" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="testSuite" sheetId="3" r:id="rId1"/>
     <sheet name="testAddCustomer" sheetId="1" r:id="rId2"/>
     <sheet name="testOpenAccount" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet1" r:id="rId8" sheetId="4"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="71">
   <si>
     <t>FirstName</t>
   </si>
@@ -72,15 +73,6 @@
     <t>H3H5B5</t>
   </si>
   <si>
-    <t>Dina</t>
-  </si>
-  <si>
-    <t>Nath</t>
-  </si>
-  <si>
-    <t>S4D6A4</t>
-  </si>
-  <si>
     <t>Raman Yanki</t>
   </si>
   <si>
@@ -144,13 +136,107 @@
     <t>y</t>
   </si>
   <si>
+    <t>TestCustomerList</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>Post Code</t>
+  </si>
+  <si>
+    <t>Account Number</t>
+  </si>
+  <si>
+    <t>Hermoine</t>
+  </si>
+  <si>
+    <t>Granger</t>
+  </si>
+  <si>
+    <t>E859AB</t>
+  </si>
+  <si>
+    <t>1001 1002 1003</t>
+  </si>
+  <si>
+    <t>Harry</t>
+  </si>
+  <si>
+    <t>Potter</t>
+  </si>
+  <si>
+    <t>E725JB</t>
+  </si>
+  <si>
+    <t>1004 1005 1006</t>
+  </si>
+  <si>
+    <t>Ron</t>
+  </si>
+  <si>
+    <t>Weasly</t>
+  </si>
+  <si>
+    <t>E55555</t>
+  </si>
+  <si>
+    <t>1007 1008 1009</t>
+  </si>
+  <si>
+    <t>Albus</t>
+  </si>
+  <si>
+    <t>Dumbledore</t>
+  </si>
+  <si>
+    <t>E55656</t>
+  </si>
+  <si>
+    <t>1010 1011 1012</t>
+  </si>
+  <si>
+    <t>Neville</t>
+  </si>
+  <si>
+    <t>Longbottom</t>
+  </si>
+  <si>
+    <t>E89898</t>
+  </si>
+  <si>
+    <t>1017 1020</t>
+  </si>
+  <si>
+    <t>1018</t>
+  </si>
+  <si>
+    <t>1019</t>
+  </si>
+  <si>
+    <t>1013 1014 1015</t>
+  </si>
+  <si>
+    <t>Runmode</t>
+  </si>
+  <si>
     <t>n</t>
+  </si>
+  <si>
+    <t>1016 1021</t>
+  </si>
+  <si>
+    <t>1022</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -160,12 +246,22 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -180,8 +276,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -476,47 +580,55 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="23.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
         <v>37</v>
-      </c>
-      <c r="B2" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
         <v>39</v>
       </c>
-      <c r="B4" t="s">
-        <v>42</v>
+      <c r="B5" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -526,18 +638,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="13.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -547,8 +659,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -558,8 +673,11 @@
       <c r="C2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -569,8 +687,11 @@
       <c r="C3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="D3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -580,8 +701,11 @@
       <c r="C4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="D4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -591,8 +715,11 @@
       <c r="C5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="D5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -602,8 +729,11 @@
       <c r="C6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="D6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -613,38 +743,36 @@
       <c r="C7" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="D7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+        <v>9</v>
+      </c>
+      <c r="D8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="B9" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" t="s">
-        <v>34</v>
+        <v>31</v>
+      </c>
+      <c r="D9" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -654,99 +782,302 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L11" sqref="G11:L21"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" customWidth="1"/>
-    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="15.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
         <v>27</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
+      <c r="C5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
         <v>22</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
-        <v>33</v>
-      </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>27</v>
+      </c>
+      <c r="C10" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.7421875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="12.23828125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.01171875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="16.2265625" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="5">
+        <v>40</v>
+      </c>
+      <c r="B1" t="s" s="6">
+        <v>41</v>
+      </c>
+      <c r="C1" t="s" s="7">
+        <v>42</v>
+      </c>
+      <c r="D1" t="s" s="8">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
first commit on 22 Dec
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -4,20 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="11415" windowHeight="8955" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="11415" windowHeight="8955"/>
   </bookViews>
   <sheets>
     <sheet name="testSuite" sheetId="3" r:id="rId1"/>
     <sheet name="testAddCustomer" sheetId="1" r:id="rId2"/>
     <sheet name="testOpenAccount" sheetId="2" r:id="rId3"/>
-    <sheet name="testDeleteCustomer" r:id="rId8" sheetId="4"/>
+    <sheet name="testDeleteCustomer" r:id="rId7" sheetId="4"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1143" uniqueCount="79">
   <si>
     <t>FirstName</t>
   </si>
@@ -139,6 +139,15 @@
     <t>TestCustomerList</t>
   </si>
   <si>
+    <t>Runmode</t>
+  </si>
+  <si>
+    <t>testDeleteCustomer</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
     <t>First Name</t>
   </si>
   <si>
@@ -151,6 +160,12 @@
     <t>Account Number</t>
   </si>
   <si>
+    <t>Delete Customer</t>
+  </si>
+  <si>
+    <t>Hermoine</t>
+  </si>
+  <si>
     <t>Granger</t>
   </si>
   <si>
@@ -172,6 +187,9 @@
     <t>1004 1005 1006</t>
   </si>
   <si>
+    <t>Ron</t>
+  </si>
+  <si>
     <t>Weasly</t>
   </si>
   <si>
@@ -181,6 +199,9 @@
     <t>1007 1008 1009</t>
   </si>
   <si>
+    <t>N</t>
+  </si>
+  <si>
     <t>Albus</t>
   </si>
   <si>
@@ -196,33 +217,15 @@
     <t>Neville</t>
   </si>
   <si>
+    <t>Longbottom</t>
+  </si>
+  <si>
     <t>E89898</t>
   </si>
   <si>
     <t>1013 1014 1015</t>
   </si>
   <si>
-    <t>Runmode</t>
-  </si>
-  <si>
-    <t>Delete Customer</t>
-  </si>
-  <si>
-    <t>Longbottom</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>testDeleteCustomer</t>
-  </si>
-  <si>
-    <t>Hermoine</t>
-  </si>
-  <si>
-    <t>Ron</t>
-  </si>
-  <si>
     <t>1016 1022</t>
   </si>
   <si>
@@ -239,6 +242,18 @@
   </si>
   <si>
     <t>1023</t>
+  </si>
+  <si>
+    <t>1016 1019</t>
+  </si>
+  <si>
+    <t>1017</t>
+  </si>
+  <si>
+    <t>1020</t>
+  </si>
+  <si>
+    <t>1022</t>
   </si>
 </sst>
 </file>
@@ -263,12 +278,12 @@
       <patternFill patternType="gray125"/>
     </fill>
     <fill>
-      <patternFill patternType="solid">
+      <patternFill patternType="none">
         <fgColor indexed="55"/>
       </patternFill>
     </fill>
     <fill>
-      <patternFill patternType="none">
+      <patternFill patternType="solid">
         <fgColor indexed="55"/>
       </patternFill>
     </fill>
@@ -285,28 +300,98 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -603,8 +688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -654,7 +739,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="B6" t="s">
         <v>38</v>
@@ -670,7 +755,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D9"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -689,7 +774,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>61</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -759,7 +844,7 @@
         <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -787,7 +872,7 @@
         <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -814,7 +899,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C10"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -908,7 +993,7 @@
         <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -954,34 +1039,34 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s" s="16">
-        <v>40</v>
-      </c>
-      <c r="B1" t="s" s="17">
-        <v>41</v>
-      </c>
-      <c r="C1" t="s" s="18">
-        <v>42</v>
-      </c>
-      <c r="D1" t="s" s="19">
+      <c r="A1" t="s" s="86">
         <v>43</v>
       </c>
-      <c r="E1" t="s" s="20">
-        <v>62</v>
+      <c r="B1" t="s" s="87">
+        <v>44</v>
+      </c>
+      <c r="C1" t="s" s="88">
+        <v>45</v>
+      </c>
+      <c r="D1" t="s" s="89">
+        <v>46</v>
+      </c>
+      <c r="E1" t="s" s="90">
+        <v>47</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="C2" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="D2" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="E2" t="s">
         <v>37</v>
@@ -989,13 +1074,16 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>53</v>
+      </c>
+      <c r="C3" t="s">
+        <v>54</v>
       </c>
       <c r="D3" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="E3" t="s">
         <v>37</v>
@@ -1003,13 +1091,16 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>67</v>
+        <v>56</v>
+      </c>
+      <c r="B4" t="s">
+        <v>57</v>
       </c>
       <c r="C4" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="D4" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="E4" t="s">
         <v>37</v>
@@ -1017,16 +1108,16 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="B5" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="C5" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="D5" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="E5" t="s">
         <v>37</v>
@@ -1034,19 +1125,19 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="B6" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C6" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="D6" t="s">
+        <v>68</v>
+      </c>
+      <c r="E6" t="s">
         <v>60</v>
-      </c>
-      <c r="E6" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="7">
@@ -1060,10 +1151,10 @@
         <v>9</v>
       </c>
       <c r="D7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E7" t="s">
-        <v>64</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8">
@@ -1077,7 +1168,7 @@
         <v>10</v>
       </c>
       <c r="D8" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E8" t="s">
         <v>37</v>
@@ -1094,10 +1185,10 @@
         <v>14</v>
       </c>
       <c r="D9" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E9" t="s">
-        <v>64</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10">
@@ -1111,10 +1202,10 @@
         <v>11</v>
       </c>
       <c r="D10" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E10" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11">
@@ -1128,7 +1219,7 @@
         <v>17</v>
       </c>
       <c r="D11" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E11" t="s">
         <v>37</v>
@@ -1145,10 +1236,10 @@
         <v>31</v>
       </c>
       <c r="D12" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E12" t="s">
-        <v>64</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>